<commit_message>
update der kampfhandlung methode
</commit_message>
<xml_diff>
--- a/data/held_elsbeth.xlsx
+++ b/data/held_elsbeth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B128E4-BA84-4B55-BAC7-BD5E639302A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339A867C-C239-4A8B-A642-EEEDB1A7A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC708954-D5BA-48F4-A0A8-28752AA467BF}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
neuer pointer für vorhandene grimoires
</commit_message>
<xml_diff>
--- a/data/held_elsbeth.xlsx
+++ b/data/held_elsbeth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaelm\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339A867C-C239-4A8B-A642-EEEDB1A7A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A18F33-2BFA-400D-A724-8326E4C29D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC708954-D5BA-48F4-A0A8-28752AA467BF}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BC708954-D5BA-48F4-A0A8-28752AA467BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>alter</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Mensch</t>
   </si>
   <si>
-    <t>heldentyp</t>
-  </si>
-  <si>
     <t>MU</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>AsP</t>
   </si>
   <si>
-    <t>Int</t>
-  </si>
-  <si>
     <t>AP</t>
   </si>
   <si>
@@ -99,6 +93,30 @@
   </si>
   <si>
     <t>Elsbeth</t>
+  </si>
+  <si>
+    <t>has_grimoire</t>
+  </si>
+  <si>
+    <t>profession</t>
+  </si>
+  <si>
+    <t>INI</t>
+  </si>
+  <si>
+    <t>KaP</t>
+  </si>
+  <si>
+    <t>ausweichen</t>
+  </si>
+  <si>
+    <t>geschwindigkeit</t>
+  </si>
+  <si>
+    <t>Schriftstellerin</t>
+  </si>
+  <si>
+    <t>beruf</t>
   </si>
 </sst>
 </file>
@@ -157,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -303,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,34 +471,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65780383-107F-4D9D-81FB-09DDAAB0CBB2}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -496,107 +516,147 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="B26" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>